<commit_message>
Updated Code & Cleaned Project Files
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ApplicationTestData.xlsx
+++ b/src/test/resources/TestData/ApplicationTestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Automation Mini Projects\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Copy Of Mini Projects\DataDrivenTestAutomationFramework\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62424714-EB9A-4379-BF44-3B6A2FF15125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C468F18-DCFA-47C4-BAC9-AEC9E51D7B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{69E161D9-8E89-4A8D-B0DE-E7E03B53B9FF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>firstName</t>
   </si>
@@ -54,181 +54,70 @@
     <t>email</t>
   </si>
   <si>
-    <t>TqTr2siS</t>
-  </si>
-  <si>
-    <t>atCz7yEh</t>
-  </si>
-  <si>
-    <t>6pAXA-,y</t>
-  </si>
-  <si>
-    <t>2608438621</t>
-  </si>
-  <si>
-    <t>Doctor</t>
-  </si>
-  <si>
-    <t>cZyRBFW3@gmail.com</t>
-  </si>
-  <si>
-    <t>Oqayj4X6</t>
-  </si>
-  <si>
-    <t>Oh98dkuF</t>
-  </si>
-  <si>
-    <t>5Xz;(:Nb</t>
-  </si>
-  <si>
-    <t>4332491953</t>
-  </si>
-  <si>
-    <t>xutXaUuD@gmail.com</t>
-  </si>
-  <si>
-    <t>KGaxYLZQ</t>
-  </si>
-  <si>
-    <t>VXZ0htRL</t>
-  </si>
-  <si>
-    <t>f90MJ%!o</t>
-  </si>
-  <si>
-    <t>4381696637</t>
+    <t>Sona</t>
+  </si>
+  <si>
+    <t>Botsford</t>
+  </si>
+  <si>
+    <t>linda.stracke@hotmail.com</t>
+  </si>
+  <si>
+    <t>1740526410</t>
   </si>
   <si>
     <t>Scientist</t>
   </si>
   <si>
-    <t>wgiTLOOu@gmail.com</t>
-  </si>
-  <si>
-    <t>3v3EYqgL</t>
-  </si>
-  <si>
-    <t>IgygkMqW</t>
-  </si>
-  <si>
-    <t>MO(eCI*3</t>
-  </si>
-  <si>
-    <t>6547056814</t>
-  </si>
-  <si>
-    <t>Engineer</t>
-  </si>
-  <si>
-    <t>KvlHYOhW@gmail.com</t>
-  </si>
-  <si>
-    <t>6BniPIg5</t>
-  </si>
-  <si>
-    <t>ACUTqfiz</t>
-  </si>
-  <si>
-    <t>X)yqC55a</t>
-  </si>
-  <si>
-    <t>8201898707</t>
-  </si>
-  <si>
-    <t>3IIcf1DU@gmail.com</t>
-  </si>
-  <si>
-    <t>Jkt1hn8Y</t>
-  </si>
-  <si>
-    <t>bjCra757</t>
-  </si>
-  <si>
-    <t>Bl?4=Z$J</t>
-  </si>
-  <si>
-    <t>9494574601</t>
+    <t>*jB8lVMF!</t>
+  </si>
+  <si>
+    <t>Agustin</t>
+  </si>
+  <si>
+    <t>King</t>
+  </si>
+  <si>
+    <t>malika.reilly@hotmail.com</t>
+  </si>
+  <si>
+    <t>5322258454</t>
   </si>
   <si>
     <t>Student</t>
   </si>
   <si>
-    <t>ohS1G2sa@gmail.com</t>
-  </si>
-  <si>
-    <t>MFCUznLW</t>
-  </si>
-  <si>
-    <t>lUjOCNej</t>
-  </si>
-  <si>
-    <t>q$MXU5zh</t>
-  </si>
-  <si>
-    <t>9140521824</t>
-  </si>
-  <si>
-    <t>2ftaaiRq@gmail.com</t>
-  </si>
-  <si>
-    <t>6ftAZYBF</t>
-  </si>
-  <si>
-    <t>9GeLX4a5</t>
-  </si>
-  <si>
-    <t>?x{7Q!AN</t>
-  </si>
-  <si>
-    <t>1297102310</t>
-  </si>
-  <si>
-    <t>84ls95yg@gmail.com</t>
-  </si>
-  <si>
-    <t>d0l7dbN8</t>
-  </si>
-  <si>
-    <t>GpijYMPi</t>
-  </si>
-  <si>
-    <t>.JfS7ZW?</t>
-  </si>
-  <si>
-    <t>4215004653</t>
-  </si>
-  <si>
-    <t>IAAPy4Ep@gmail.com</t>
-  </si>
-  <si>
-    <t>5OIst7ir</t>
-  </si>
-  <si>
-    <t>33VBdMmG</t>
-  </si>
-  <si>
-    <t>w&lt;M9|mX*</t>
-  </si>
-  <si>
-    <t>6827319822</t>
-  </si>
-  <si>
-    <t>C6KK4Y65@gmail.com</t>
-  </si>
-  <si>
-    <t>GmmBhw19</t>
-  </si>
-  <si>
-    <t>wlchb3tZ</t>
-  </si>
-  <si>
-    <t>$3vkvN^)</t>
-  </si>
-  <si>
-    <t>5777987600</t>
-  </si>
-  <si>
-    <t>AcWhB6vZ@gmail.com</t>
+    <t>S7$HM^Lz</t>
+  </si>
+  <si>
+    <t>Luciano</t>
+  </si>
+  <si>
+    <t>Goyette</t>
+  </si>
+  <si>
+    <t>reuben.boehm@yahoo.com</t>
+  </si>
+  <si>
+    <t>3770895225</t>
+  </si>
+  <si>
+    <t>@fSv%180A</t>
+  </si>
+  <si>
+    <t>Len</t>
+  </si>
+  <si>
+    <t>Kemmer</t>
+  </si>
+  <si>
+    <t>destiny.block@yahoo.com</t>
+  </si>
+  <si>
+    <t>1542678495</t>
+  </si>
+  <si>
+    <t>8$fEA#%$</t>
   </si>
 </sst>
 </file>
@@ -597,20 +486,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC6BBCE9-8EFC-4485-B036-F79971E5BE8E}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="14.28515625"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="12.7109375"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.0"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="25.85546875"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="17.140625"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="15.7109375"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="22.42578125"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" x14ac:dyDescent="0.25">
@@ -621,7 +510,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
@@ -630,7 +519,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -653,7 +542,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s" s="0">
         <v>12</v>
       </c>
@@ -667,33 +556,33 @@
         <v>15</v>
       </c>
       <c r="E3" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s" s="0">
         <v>10</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>21</v>
       </c>
       <c r="F4" t="s" s="0">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s" s="0">
         <v>23</v>
       </c>
@@ -707,150 +596,10 @@
         <v>26</v>
       </c>
       <c r="E5" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F5" t="s" s="0">
         <v>27</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s" s="0">
-        <v>29</v>
-      </c>
-      <c r="B6" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s" s="0">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s" s="0">
-        <v>35</v>
-      </c>
-      <c r="C7" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="D7" t="s" s="0">
-        <v>37</v>
-      </c>
-      <c r="E7" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s" s="0">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s" s="0">
-        <v>40</v>
-      </c>
-      <c r="B8" t="s" s="0">
-        <v>41</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>42</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="B9" t="s" s="0">
-        <v>46</v>
-      </c>
-      <c r="C9" t="s" s="0">
-        <v>47</v>
-      </c>
-      <c r="D9" t="s" s="0">
-        <v>48</v>
-      </c>
-      <c r="E9" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="F9" t="s" s="0">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s" s="0">
-        <v>50</v>
-      </c>
-      <c r="B10" t="s" s="0">
-        <v>51</v>
-      </c>
-      <c r="C10" t="s" s="0">
-        <v>52</v>
-      </c>
-      <c r="D10" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="E10" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F10" t="s" s="0">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s" s="0">
-        <v>55</v>
-      </c>
-      <c r="B11" t="s" s="0">
-        <v>56</v>
-      </c>
-      <c r="C11" t="s" s="0">
-        <v>57</v>
-      </c>
-      <c r="D11" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="E11" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="F11" t="s" s="0">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="B12" t="s" s="0">
-        <v>61</v>
-      </c>
-      <c r="C12" t="s" s="0">
-        <v>62</v>
-      </c>
-      <c r="D12" t="s" s="0">
-        <v>63</v>
-      </c>
-      <c r="E12" t="s" s="0">
-        <v>27</v>
-      </c>
-      <c r="F12" t="s" s="0">
-        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added : Parameterzied Tests with JUnit
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ApplicationTestData.xlsx
+++ b/src/test/resources/TestData/ApplicationTestData.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>firstName</t>
   </si>
@@ -118,6 +118,39 @@
   </si>
   <si>
     <t>8$fEA#%$</t>
+  </si>
+  <si>
+    <t>Clarence</t>
+  </si>
+  <si>
+    <t>Kuhn</t>
+  </si>
+  <si>
+    <t>vanita.romaguera@hotmail.com</t>
+  </si>
+  <si>
+    <t>5097499366</t>
+  </si>
+  <si>
+    <t>t%iye7M%y</t>
+  </si>
+  <si>
+    <t>Jenifer</t>
+  </si>
+  <si>
+    <t>VonRueden</t>
+  </si>
+  <si>
+    <t>clark.harris@yahoo.com</t>
+  </si>
+  <si>
+    <t>9898922868</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>oi$g#7Pi</t>
   </si>
 </sst>
 </file>
@@ -486,7 +519,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC6BBCE9-8EFC-4485-B036-F79971E5BE8E}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -602,6 +635,46 @@
         <v>27</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Login Test yaml
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ApplicationTestData.xlsx
+++ b/src/test/resources/TestData/ApplicationTestData.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="60">
   <si>
     <t>firstName</t>
   </si>
@@ -199,6 +199,21 @@
   </si>
   <si>
     <t>h8vnm13M!</t>
+  </si>
+  <si>
+    <t>Delbert</t>
+  </si>
+  <si>
+    <t>Parker</t>
+  </si>
+  <si>
+    <t>ronald.kshlerin@yahoo.com</t>
+  </si>
+  <si>
+    <t>6056110055</t>
+  </si>
+  <si>
+    <t>4rZFBc65</t>
   </si>
 </sst>
 </file>
@@ -567,7 +582,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC6BBCE9-8EFC-4485-B036-F79971E5BE8E}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
@@ -783,6 +798,26 @@
         <v>54</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s" s="0">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>